<commit_message>
BAP-19074: Remove sensio/generator-bundle package - xlsx file reader
</commit_message>
<xml_diff>
--- a/src/Oro/Bundle/ImportExportBundle/Tests/Unit/Reader/fixtures/mock_file_for_initialize.xlsx
+++ b/src/Oro/Bundle/ImportExportBundle/Tests/Unit/Reader/fixtures/mock_file_for_initialize.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -62,14 +62,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -129,7 +131,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -151,77 +161,77 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:D8"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
BAP-19082: Update liuggio/excelbundle package (#24480)
* BAP-19082: Update liuggio/excelbundle package
- add cache provider whit store data in "php://temp"
- change XLSX write from "PHPExcel" to "PhpOffice\PhpSpreadsheet"
- added psr exception on invalid arguments for php temp cache implementation
- update xlsx writer test
- change package to read/write xlsx to "box/spout"
- update dependencies list
- remove missing bundle initialization
- remove "php://temp" cache
- added SymfonyRequirements.php to git
- ignoring coding standards in SymfonyRequirements.php
* Restore XSS tests to original flow
</commit_message>
<xml_diff>
--- a/src/Oro/Bundle/ImportExportBundle/Tests/Unit/Reader/fixtures/mock_file_for_initialize.xlsx
+++ b/src/Oro/Bundle/ImportExportBundle/Tests/Unit/Reader/fixtures/mock_file_for_initialize.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -62,14 +62,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -129,7 +131,15 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -151,77 +161,77 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A4:D8"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A5" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>